<commit_message>
debug of threshold: noted python is 7 orders of magnitude larger than working matlab!
</commit_message>
<xml_diff>
--- a/camparam.xlsx
+++ b/camparam.xlsx
@@ -179,7 +179,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -236,10 +236,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -250,7 +250,7 @@
         <v>2900</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>3500</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,10 +340,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0.1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,10 +351,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>10</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
big fix to smoothness parameter
</commit_message>
<xml_diff>
--- a/camparam.xlsx
+++ b/camparam.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="502" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="713" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>camserial</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>medfiltsize</t>
+  </si>
+  <si>
+    <t>trimedgeof</t>
+  </si>
+  <si>
+    <t>openradius</t>
+  </si>
+  <si>
+    <t>closewidth</t>
+  </si>
+  <si>
+    <t>closeheight</t>
   </si>
 </sst>
 </file>
@@ -176,10 +188,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -250,7 +262,7 @@
         <v>2900</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>6500</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,6 +389,50 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to get videowriter to work. No file written. Try imwrite instead?
</commit_message>
<xml_diff>
--- a/camparam.xlsx
+++ b/camparam.xlsx
@@ -29,8 +29,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Suggest 3. Must be ODD.
-</t>
+          <t xml:space="preserve">Suggest 3. Must be ODD.</t>
         </r>
       </text>
     </comment>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>camserial</t>
   </si>
@@ -65,21 +64,12 @@
     <t>cmax</t>
   </si>
   <si>
-    <t>fries  3d idl</t>
-  </si>
-  <si>
     <t>wienernhood</t>
   </si>
   <si>
-    <t>ian mcdaid</t>
-  </si>
-  <si>
     <t>xpix</t>
   </si>
   <si>
-    <t>jeff dome</t>
-  </si>
-  <si>
     <t>ypix</t>
   </si>
   <si>
@@ -93,9 +83,6 @@
   </si>
   <si>
     <t>maxblobarea</t>
-  </si>
-  <si>
-    <t>books: particles, field</t>
   </si>
   <si>
     <t>maxblobcount</t>
@@ -227,10 +214,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -314,21 +301,15 @@
       <c r="C7" s="0" t="n">
         <v>45000</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>512</v>
@@ -336,13 +317,10 @@
       <c r="C9" s="0" t="n">
         <v>512</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>512</v>
@@ -353,7 +331,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -364,7 +342,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -375,7 +353,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1000</v>
@@ -386,7 +364,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>100000</v>
@@ -394,13 +372,10 @@
       <c r="C14" s="0" t="n">
         <v>100000</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>10</v>
@@ -411,7 +386,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>2</v>
@@ -422,7 +397,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>10000</v>
@@ -433,18 +408,18 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>3</v>
@@ -455,7 +430,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>5</v>
@@ -466,7 +441,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
@@ -477,7 +452,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>5</v>
@@ -488,7 +463,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
implemented excellent working GMM code
</commit_message>
<xml_diff>
--- a/camparam.xlsx
+++ b/camparam.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="976" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,9 @@
             <charset val="1"/>
           </rPr>
           <t>hs: Horn-Schunck (opencv2 only)
-farneback: Farneback method</t>
+farneback: Farneback method
+mog: background subtractor (opencv2 only)
+mog2: background subtractor</t>
         </r>
       </text>
     </comment>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>camserial</t>
   </si>
@@ -60,7 +62,7 @@
     <t>ofmethod</t>
   </si>
   <si>
-    <t>farneback</t>
+    <t>mog2</t>
   </si>
   <si>
     <t>hssmooth</t>
@@ -130,6 +132,15 @@
   </si>
   <si>
     <t>closeheight</t>
+  </si>
+  <si>
+    <t>nhistory</t>
+  </si>
+  <si>
+    <t>nmixtures</t>
+  </si>
+  <si>
+    <t>varThreshold</t>
   </si>
 </sst>
 </file>
@@ -231,10 +242,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -497,6 +508,39 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
messages re methods unavailable
</commit_message>
<xml_diff>
--- a/camparam.xlsx
+++ b/camparam.xlsx
@@ -62,12 +62,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="A29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Default 0.05
+Grimson-Stauffer 0.0</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>camserial</t>
   </si>
@@ -75,7 +89,7 @@
     <t>ofmethod</t>
   </si>
   <si>
-    <t>mog2</t>
+    <t>gmg</t>
   </si>
   <si>
     <t>hssmooth</t>
@@ -154,6 +168,9 @@
   </si>
   <si>
     <t>varThreshold</t>
+  </si>
+  <si>
+    <t>CompResThres</t>
   </si>
 </sst>
 </file>
@@ -255,15 +272,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,6 +573,17 @@
       </c>
       <c r="C28" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hdf5 and fits video reader
</commit_message>
<xml_diff>
--- a/camparam.xlsx
+++ b/camparam.xlsx
@@ -5,12 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -82,12 +87,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>camserial</t>
   </si>
   <si>
     <t>ofmethod</t>
+  </si>
+  <si>
+    <t>farneback</t>
   </si>
   <si>
     <t>hs</t>
@@ -281,8 +289,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,12 +312,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.001</v>
@@ -320,7 +328,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -331,7 +339,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -342,7 +350,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>900</v>
@@ -353,7 +361,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2900</v>
@@ -364,12 +372,12 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>512</v>
@@ -380,7 +388,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>512</v>
@@ -391,7 +399,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -402,7 +410,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -413,7 +421,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1000</v>
@@ -424,7 +432,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>100000</v>
@@ -435,7 +443,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>10</v>
@@ -446,7 +454,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>50</v>
@@ -457,7 +465,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2</v>
@@ -468,7 +476,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>10000</v>
@@ -479,18 +487,18 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
@@ -501,7 +509,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>5</v>
@@ -512,7 +520,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>3</v>
@@ -523,7 +531,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>5</v>
@@ -534,7 +542,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
@@ -545,7 +553,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>100</v>
@@ -556,7 +564,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>5</v>
@@ -567,7 +575,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
@@ -578,7 +586,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.05</v>

</xml_diff>